<commit_message>
Initial Skill creation & conversion.
Mapping NWN skills to the most similar d20 Modern Skills & adding the rest.
</commit_message>
<xml_diff>
--- a/TEXT/GW Skill Mapping.xlsx
+++ b/TEXT/GW Skill Mapping.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -353,6 +351,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1572,10 +1571,10 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2487,28 +2486,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>